<commit_message>
add gitignore word, excel, powerpoint
</commit_message>
<xml_diff>
--- a/Bảng báo các tiến độ công việc.xlsx
+++ b/Bảng báo các tiến độ công việc.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK7\TLCN\NhaTroSV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD4B9A-C28F-49F4-813A-ADDCF956BFC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Tuần</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +75,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +360,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bo sung bao cao
</commit_message>
<xml_diff>
--- a/Bảng báo các tiến độ công việc.xlsx
+++ b/Bảng báo các tiến độ công việc.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK7\TLCN\NhaTroSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TLCN\NhaTroSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E996CF-3EC8-47A9-82A8-8906EBF435E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Tuần</t>
   </si>
@@ -72,12 +71,19 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Thọ: Giao diện phần app.
+Công: Giao diện phần web API.</t>
+  </si>
+  <si>
+    <t>Hoàn thành xong giao diện.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,11 +414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -494,20 +500,25 @@
         <v>43738</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C10" si="0">C3+14</f>
+        <f t="shared" ref="C4:C9" si="0">C3+14</f>
         <v>43751</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" ref="B5:B10" si="1">B4+14</f>
+        <f t="shared" ref="B5:B9" si="1">B4+14</f>
         <v>43752</v>
       </c>
       <c r="C5" s="3">

</xml_diff>

<commit_message>
update cong viec den 27/10
</commit_message>
<xml_diff>
--- a/Bảng báo các tiến độ công việc.xlsx
+++ b/Bảng báo các tiến độ công việc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TLCN\NhaTroSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK7\TLCN\NhaTroSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7781609-6293-4685-AEBA-291C8ECAE9AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Tuần</t>
   </si>
@@ -66,24 +67,27 @@
     <t>Hoàn thiện usecase, vẽ sequence diagram, class diagram, lược đồ csdl, thiết kế UI(thiết kế UI, danh sách xử lý, sơ đồ luồng, thuật toán)</t>
   </si>
   <si>
-    <t>Thầy: sửa usecase, sequence, class, csdl, UI
-Team: Hoàn thiện thiết kế giao diện, xong r code</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
+    <t>hoàn thành usecase, sequence, class diagram, lược đồ csdl, prototype</t>
+  </si>
+  <si>
+    <t>thiết kế UI cho app, web, viết api</t>
+  </si>
+  <si>
     <t>Thọ: Giao diện phần app.
-Công: Giao diện phần web API.</t>
-  </si>
-  <si>
-    <t>Hoàn thành xong giao diện.</t>
+Công: Giao diện phần web, viết API.</t>
+  </si>
+  <si>
+    <t>Hoàn thành xong giao diện web
+App: hoàn thành giao diện main, login, person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,11 +418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -426,7 +430,7 @@
     <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
     <col min="2" max="3" width="21.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="58.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="47" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -444,7 +448,7 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -464,10 +468,10 @@
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -486,12 +490,14 @@
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="54" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -504,16 +510,16 @@
         <v>43751</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -526,9 +532,12 @@
         <v>43765</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -543,9 +552,10 @@
         <v>43779</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
@@ -560,9 +570,10 @@
         <v>43793</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
@@ -577,7 +588,8 @@
         <v>43807</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
@@ -592,28 +604,29 @@
         <v>43821</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>